<commit_message>
excel colores, FIX login error
</commit_message>
<xml_diff>
--- a/out.xlsx
+++ b/out.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="47">
   <si>
     <t>PROCESO</t>
   </si>
@@ -40,7 +40,7 @@
     <t>CRITERIOS PARA ESTABLECER CONTROLES</t>
   </si>
   <si>
-    <t>MEDIDAS DE CONTROL</t>
+    <t>MEDIDAS DE CONTROL A IMPLEMENTAR</t>
   </si>
   <si>
     <t>FUENTE</t>
@@ -85,6 +85,54 @@
     <t>EXISTENCIA DE REQUISITOS LEGALES ASOCIADOS</t>
   </si>
   <si>
+    <t>Gerente General</t>
+  </si>
+  <si>
+    <t>Oficina de gerente general</t>
+  </si>
+  <si>
+    <t>SSS</t>
+  </si>
+  <si>
+    <t>Postura prolongada</t>
+  </si>
+  <si>
+    <t>SSSS</t>
+  </si>
+  <si>
+    <t>Programa de pausas activas</t>
+  </si>
+  <si>
+    <t>N.A.</t>
+  </si>
+  <si>
+    <t>Capacitación al personal en autocuidado. Capacitación en higiene postural</t>
+  </si>
+  <si>
+    <t>Medio</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> No aceptable</t>
+  </si>
+  <si>
+    <t>ZZZZZ</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>DD</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>SDSDSD</t>
+  </si>
+  <si>
     <t>Subgerente</t>
   </si>
   <si>
@@ -94,61 +142,16 @@
     <t>DDD</t>
   </si>
   <si>
-    <t>Postura prolongada</t>
-  </si>
-  <si>
     <t>DDDD</t>
   </si>
   <si>
-    <t>Programa de pausas activas</t>
-  </si>
-  <si>
-    <t>N.A.</t>
-  </si>
-  <si>
-    <t>Capacitación al personal en autocuidado. Capacitación en higiene postural</t>
-  </si>
-  <si>
-    <t>Medio</t>
-  </si>
-  <si>
     <t>II</t>
   </si>
   <si>
     <t>Aceptable con control específico</t>
   </si>
   <si>
-    <t>NO</t>
-  </si>
-  <si>
-    <t>DD</t>
-  </si>
-  <si>
-    <t>Gerente General</t>
-  </si>
-  <si>
-    <t>Oficina de gerente general</t>
-  </si>
-  <si>
-    <t>SSS</t>
-  </si>
-  <si>
-    <t>SSSS</t>
-  </si>
-  <si>
-    <t>I</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> No aceptable</t>
-  </si>
-  <si>
-    <t>ZZZZZ</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>SDSDSD</t>
+    <t>Aceptable</t>
   </si>
 </sst>
 </file>
@@ -170,7 +173,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -187,6 +190,24 @@
       <patternFill patternType="darkTrellis">
         <fgColor rgb="FF9900"/>
         <bgColor rgb="FF9900"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="darkTrellis">
+        <fgColor rgb="FF0000"/>
+        <bgColor rgb="FF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="darkTrellis">
+        <fgColor rgb="FFA500"/>
+        <bgColor rgb="FFA500"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="darkTrellis">
+        <fgColor rgb="008000"/>
+        <bgColor rgb="008000"/>
       </patternFill>
     </fill>
   </fills>
@@ -209,7 +230,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -221,6 +242,9 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -560,7 +584,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V4"/>
+  <dimension ref="A1:V5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="22" width="25" customWidth="1"/>
@@ -706,51 +730,51 @@
         <v>32</v>
       </c>
       <c r="M3">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="N3">
-        <v>150</v>
+        <v>600</v>
       </c>
       <c r="O3" t="s">
         <v>33</v>
       </c>
-      <c r="P3" t="s">
+      <c r="P3" s="5" t="s">
         <v>34</v>
       </c>
       <c r="Q3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R3" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="S3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="T3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="U3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="V3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D4" t="s">
         <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F4" t="s">
         <v>29</v>
@@ -774,34 +798,102 @@
         <v>32</v>
       </c>
       <c r="M4">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="N4">
-        <v>600</v>
+        <v>150</v>
       </c>
       <c r="O4" t="s">
-        <v>41</v>
-      </c>
-      <c r="P4" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="Q4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R4" t="s">
         <v>43</v>
       </c>
       <c r="S4" t="s">
+        <v>36</v>
+      </c>
+      <c r="T4" t="s">
+        <v>37</v>
+      </c>
+      <c r="U4" t="s">
+        <v>37</v>
+      </c>
+      <c r="V4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <v>3</v>
+      </c>
+      <c r="K5">
+        <v>6</v>
+      </c>
+      <c r="L5" t="s">
+        <v>32</v>
+      </c>
+      <c r="M5">
+        <v>100</v>
+      </c>
+      <c r="N5">
+        <v>600</v>
+      </c>
+      <c r="O5" t="s">
+        <v>33</v>
+      </c>
+      <c r="P5" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5" t="s">
         <v>35</v>
       </c>
-      <c r="T4" t="s">
+      <c r="S5" t="s">
         <v>36</v>
       </c>
-      <c r="U4" t="s">
-        <v>44</v>
-      </c>
-      <c r="V4" t="s">
-        <v>45</v>
+      <c r="T5" t="s">
+        <v>37</v>
+      </c>
+      <c r="U5" t="s">
+        <v>38</v>
+      </c>
+      <c r="V5" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>